<commit_message>
experiments table sorted by categories
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jollopre/repositories/Dropbox/KTP_docs/XML/SSM/experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jollopre/repositories/ssm/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$D$42:$F$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$D$24:$F$55</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Survey</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Randomising</t>
+  </si>
+  <si>
+    <t>Rotating</t>
+  </si>
+  <si>
+    <t>Feature</t>
   </si>
 </sst>
 </file>
@@ -471,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="Q36" sqref="A22:Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1314,500 +1323,610 @@
         <v>34</v>
       </c>
     </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>16</v>
+      </c>
+      <c r="F23">
+        <v>11</v>
+      </c>
+      <c r="G23">
+        <v>8</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>9</v>
+      </c>
+      <c r="L23">
+        <v>3</v>
+      </c>
+      <c r="M23">
+        <v>9</v>
+      </c>
+      <c r="N23">
+        <v>4</v>
+      </c>
+      <c r="O23">
+        <v>9</v>
+      </c>
+      <c r="P23">
+        <v>11</v>
+      </c>
+      <c r="Q23" s="1">
+        <f>SUM(B23:P23)</f>
+        <v>126</v>
+      </c>
+    </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>36</v>
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>11</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>6</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>12</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+      <c r="N24">
+        <v>6</v>
+      </c>
+      <c r="O24">
+        <v>9</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="1">
+        <f>SUM(B24:P24)</f>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P25">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q25" s="1">
-        <f t="shared" ref="Q25:Q38" si="1">SUM(B25:P25)</f>
-        <v>0</v>
+        <f>SUM(B25:P25)</f>
+        <v>53</v>
       </c>
       <c r="V25" s="1"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>SUM(B26:P26)</f>
+        <v>33</v>
       </c>
       <c r="V26" s="1"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J27">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>5</v>
+      </c>
+      <c r="N27">
         <v>6</v>
       </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>5</v>
-      </c>
       <c r="O27">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P27">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q27" s="1">
-        <f t="shared" si="1"/>
-        <v>51</v>
+        <f>SUM(B27:P27)</f>
+        <v>32</v>
       </c>
       <c r="V27" s="1"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J28">
         <v>1</v>
       </c>
       <c r="K28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M28">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O28">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="P28">
         <v>1</v>
       </c>
       <c r="Q28" s="1">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <f>SUM(B28:P28)</f>
+        <v>19</v>
       </c>
       <c r="V28" s="1"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="J29">
+        <v>9</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <v>6</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
         <v>5</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>2</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <v>2</v>
-      </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>3</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
       <c r="O29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P29">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q29" s="1">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f>SUM(B29:P29)</f>
+        <v>51</v>
       </c>
       <c r="V29" s="1"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J30">
         <v>2</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L30">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q30" s="1">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f>SUM(B30:P30)</f>
+        <v>43</v>
       </c>
       <c r="V30" s="1"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
         <v>6</v>
       </c>
-      <c r="J31">
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1">
+        <f>SUM(B31:P31)</f>
         <v>8</v>
-      </c>
-      <c r="K31">
-        <v>3</v>
-      </c>
-      <c r="L31">
-        <v>8</v>
-      </c>
-      <c r="M31">
-        <v>2</v>
-      </c>
-      <c r="N31">
-        <v>1</v>
-      </c>
-      <c r="O31">
-        <v>7</v>
-      </c>
-      <c r="P31">
-        <v>8</v>
-      </c>
-      <c r="Q31" s="1">
-        <f t="shared" si="1"/>
-        <v>53</v>
       </c>
       <c r="V31" s="1"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B32">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
       <c r="L32">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="M32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O32">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="P32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="1">
-        <f t="shared" si="1"/>
-        <v>78</v>
+        <f>SUM(B32:P32)</f>
+        <v>4</v>
       </c>
       <c r="V32" s="1"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1816,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1831,10 +1950,10 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -1846,23 +1965,23 @@
         <v>0</v>
       </c>
       <c r="N33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33">
         <v>0</v>
       </c>
       <c r="P33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="1">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f>SUM(B33:P33)</f>
+        <v>0</v>
       </c>
       <c r="V33" s="1"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1871,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1886,10 +2005,10 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -1901,23 +2020,23 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
       <c r="P34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q34" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>SUM(B34:P34)</f>
+        <v>22</v>
       </c>
       <c r="V34" s="1"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1944,7 +2063,7 @@
         <v>2</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -1962,217 +2081,74 @@
         <v>0</v>
       </c>
       <c r="P35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q35" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>SUM(B35:P35)</f>
+        <v>6</v>
       </c>
       <c r="V35" s="1"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K36">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q36" s="1">
-        <f t="shared" si="1"/>
-        <v>33</v>
+        <f>SUM(B36:P36)</f>
+        <v>4</v>
       </c>
       <c r="V36" s="1"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37">
-        <v>8</v>
-      </c>
-      <c r="C37">
-        <v>10</v>
-      </c>
-      <c r="D37">
-        <v>7</v>
-      </c>
-      <c r="E37">
-        <v>16</v>
-      </c>
-      <c r="F37">
-        <v>11</v>
-      </c>
-      <c r="G37">
-        <v>8</v>
-      </c>
-      <c r="H37">
-        <v>10</v>
-      </c>
-      <c r="I37">
-        <v>9</v>
-      </c>
-      <c r="J37">
-        <v>2</v>
-      </c>
-      <c r="K37">
-        <v>9</v>
-      </c>
-      <c r="L37">
-        <v>3</v>
-      </c>
-      <c r="M37">
-        <v>9</v>
-      </c>
-      <c r="N37">
-        <v>4</v>
-      </c>
-      <c r="O37">
-        <v>9</v>
-      </c>
-      <c r="P37">
-        <v>11</v>
-      </c>
-      <c r="Q37" s="1">
-        <f t="shared" si="1"/>
-        <v>126</v>
-      </c>
       <c r="V37" s="1"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>4</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <v>5</v>
-      </c>
-      <c r="H38">
-        <v>4</v>
-      </c>
-      <c r="I38">
-        <v>2</v>
-      </c>
-      <c r="J38">
-        <v>2</v>
-      </c>
-      <c r="K38">
-        <v>4</v>
-      </c>
-      <c r="L38">
-        <v>2</v>
-      </c>
-      <c r="M38">
-        <v>4</v>
-      </c>
-      <c r="N38">
-        <v>1</v>
-      </c>
-      <c r="O38">
-        <v>1</v>
-      </c>
-      <c r="P38">
-        <v>5</v>
-      </c>
-      <c r="Q38" s="1">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
       <c r="V38" s="1"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F54" s="1"/>
     </row>
     <row r="55" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F55" s="1"/>

</xml_diff>